<commit_message>
Updated timecard (3/25/19), worked on GUI for an hour
</commit_message>
<xml_diff>
--- a/time_cards.xlsx
+++ b/time_cards.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Desktop\C.A.R\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AndrewCase/Repositories/C.A.R./"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8BDCB7-4770-4782-9D96-D77C8FE5441E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD2E64B1-C6BD-1D41-9336-C619A886A4FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22700" windowHeight="14280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -72,17 +72,17 @@
     <t>15h 37m</t>
   </si>
   <si>
-    <t>17h 30m</t>
-  </si>
-  <si>
     <t>14h 14m</t>
+  </si>
+  <si>
+    <t>18h 30m</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -448,20 +448,20 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="18.3984375" customWidth="1"/>
+    <col min="1" max="2" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2" ht="16">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -469,15 +469,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -485,7 +485,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -493,7 +493,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -501,7 +501,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -509,15 +509,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
     </row>

</xml_diff>

<commit_message>
Worked another hour on GUI
</commit_message>
<xml_diff>
--- a/time_cards.xlsx
+++ b/time_cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AndrewCase/Repositories/C.A.R./"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD2E64B1-C6BD-1D41-9336-C619A886A4FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A594BB-03E9-0F44-ACB6-CB2A6770F19F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="22700" windowHeight="14280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,7 +75,7 @@
     <t>14h 14m</t>
   </si>
   <si>
-    <t>18h 30m</t>
+    <t>19h 30m</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Updated timecards (Matt +2hours, Weston +4hours, Mine+4hours)
</commit_message>
<xml_diff>
--- a/time_cards.xlsx
+++ b/time_cards.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\burto\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AndrewCase/Repositories/C.A.R./"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0C8BA84-0622-4072-86A9-9BCDDCFE47A5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7252FCD-02CF-104D-BD2C-03D0E0582B2C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1103" yWindow="915" windowWidth="9922" windowHeight="12765" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -66,23 +66,23 @@
     <t>19h 37m</t>
   </si>
   <si>
-    <t>16h 15m</t>
-  </si>
-  <si>
-    <t>19h 14m</t>
-  </si>
-  <si>
-    <t>29h 29m</t>
-  </si>
-  <si>
     <t>16h 30m</t>
+  </si>
+  <si>
+    <t>33h 29m</t>
+  </si>
+  <si>
+    <t>23h 14m</t>
+  </si>
+  <si>
+    <t>18h 15m</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -448,20 +448,20 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2" ht="16">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -469,23 +469,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -493,15 +493,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -509,15 +509,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
     </row>

</xml_diff>

<commit_message>
Adjusted my time card
</commit_message>
<xml_diff>
--- a/time_cards.xlsx
+++ b/time_cards.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AndrewCase/Repositories/C.A.R./"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stevie_damrel/Desktop/temp/C.A.R./"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7252FCD-02CF-104D-BD2C-03D0E0582B2C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9657BB55-2F5A-3243-AA87-C8ADDF2E58A7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,9 +57,6 @@
     <t>Weston Straw</t>
   </si>
   <si>
-    <t>8h 17m</t>
-  </si>
-  <si>
     <t>Iteration 2 Timecards</t>
   </si>
   <si>
@@ -76,13 +73,16 @@
   </si>
   <si>
     <t>18h 15m</t>
+  </si>
+  <si>
+    <t>13h 30m</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -448,20 +448,20 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16">
+    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -469,55 +469,55 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
     </row>

</xml_diff>

<commit_message>
Updating website and timecard
</commit_message>
<xml_diff>
--- a/time_cards.xlsx
+++ b/time_cards.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\burto\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\C.A.R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC3BD0C-0DCD-4BB0-BEC3-E0F090113967}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEDD2700-46E2-4B06-99C1-755748592AB3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="503" yWindow="315" windowWidth="9922" windowHeight="12765" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -60,9 +60,6 @@
     <t>Iteration 2 Timecards</t>
   </si>
   <si>
-    <t>19h 37m</t>
-  </si>
-  <si>
     <t>33h 29m</t>
   </si>
   <si>
@@ -76,6 +73,9 @@
   </si>
   <si>
     <t>19h 30m</t>
+  </si>
+  <si>
+    <t>22h 37m</t>
   </si>
 </sst>
 </file>
@@ -448,20 +448,20 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="18.33203125" customWidth="1"/>
+    <col min="1" max="2" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -469,55 +469,55 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
     </row>

</xml_diff>

<commit_message>
Updated timecard (+30min) - added issues and such
</commit_message>
<xml_diff>
--- a/time_cards.xlsx
+++ b/time_cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AndrewCase/Repositories/C.A.R./"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10F33D8E-7B0D-F145-906E-2939A0D97EE5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC83B8B6-AFC7-F14D-8B82-928D054F74EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -75,7 +75,7 @@
     <t>27h 14m</t>
   </si>
   <si>
-    <t>37h 00m</t>
+    <t>37h 30m</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Updated timecard (4-7-19), +11 hours from this weekend working on code
</commit_message>
<xml_diff>
--- a/time_cards.xlsx
+++ b/time_cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AndrewCase/Repositories/C.A.R./"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F367D9-CADC-E549-9F95-52EEBFAB1A70}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{882E5AD5-3718-5A46-BEB8-FC119B77843B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,7 +75,7 @@
     <t>27h 14m</t>
   </si>
   <si>
-    <t>38h 15m</t>
+    <t>49h 15m</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Added +15 min for Diagrams
</commit_message>
<xml_diff>
--- a/time_cards.xlsx
+++ b/time_cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AndrewCase/Repositories/C.A.R./"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{882E5AD5-3718-5A46-BEB8-FC119B77843B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38FB9466-2387-E941-86DF-F9C65B10B20E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,7 +75,7 @@
     <t>27h 14m</t>
   </si>
   <si>
-    <t>49h 15m</t>
+    <t>49h 30m</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Updated timecards with +1 hour for Maggie
</commit_message>
<xml_diff>
--- a/time_cards.xlsx
+++ b/time_cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AndrewCase/Repositories/C.A.R./"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38FB9466-2387-E941-86DF-F9C65B10B20E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8772CF6F-1613-E34A-83DD-6D112AAE8F45}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,9 +60,6 @@
     <t>Iteration 2 Timecards</t>
   </si>
   <si>
-    <t>19h 30m</t>
-  </si>
-  <si>
     <t>22h 37m</t>
   </si>
   <si>
@@ -76,6 +73,9 @@
   </si>
   <si>
     <t>49h 30m</t>
+  </si>
+  <si>
+    <t>20h 30m</t>
   </si>
 </sst>
 </file>
@@ -448,7 +448,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -474,7 +474,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -482,7 +482,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -490,7 +490,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -498,7 +498,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -506,7 +506,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -514,7 +514,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:2">

</xml_diff>

<commit_message>
+1:45 hours for Maggie
</commit_message>
<xml_diff>
--- a/time_cards.xlsx
+++ b/time_cards.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stevie_damrel/Desktop/Time card/C.A.R./"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AndrewCase/Repositories/C.A.R./"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4961B7A9-372A-4341-B72F-512503140F1F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F7072D-EA7A-1C46-BCD7-3D98C8C5F7A2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -66,9 +66,6 @@
     <t>27h 14m</t>
   </si>
   <si>
-    <t>20h 30m</t>
-  </si>
-  <si>
     <t>24h 45m</t>
   </si>
   <si>
@@ -76,13 +73,16 @@
   </si>
   <si>
     <t>19h 30m</t>
+  </si>
+  <si>
+    <t>21h 45m</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -448,20 +448,20 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="16">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -469,23 +469,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -493,23 +493,23 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -517,7 +517,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
     </row>

</xml_diff>

<commit_message>
Updated for Andrew and Matt
</commit_message>
<xml_diff>
--- a/time_cards.xlsx
+++ b/time_cards.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AndrewCase/Repositories/C.A.R./"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/Desktop/Code/CSI-3471/Project/C.A.R./"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F7072D-EA7A-1C46-BCD7-3D98C8C5F7A2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A33A15-1C6B-344D-A5F8-4B336200FBE1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,23 +66,23 @@
     <t>27h 14m</t>
   </si>
   <si>
-    <t>24h 45m</t>
-  </si>
-  <si>
-    <t>52h 00m</t>
-  </si>
-  <si>
     <t>19h 30m</t>
   </si>
   <si>
     <t>21h 45m</t>
+  </si>
+  <si>
+    <t>28h 50m</t>
+  </si>
+  <si>
+    <t>56h 30m</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -448,20 +448,20 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16">
+    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -469,23 +469,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -493,23 +493,23 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -517,7 +517,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
     </row>

</xml_diff>

<commit_message>
Updated time card & removed the edit ability of history and active rentals
</commit_message>
<xml_diff>
--- a/time_cards.xlsx
+++ b/time_cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AndrewCase/Repositories/C.A.R./"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6227E79-AEEC-9F4C-90DB-4E9C487F594F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A81D53CD-550C-FA4A-84A5-1AA59167005C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,7 +75,7 @@
     <t>28h 50m</t>
   </si>
   <si>
-    <t>57h 00m</t>
+    <t>57h 10m</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Added +1 hours for me & Matt
</commit_message>
<xml_diff>
--- a/time_cards.xlsx
+++ b/time_cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AndrewCase/Repositories/C.A.R./"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B400C25-A1F0-944A-B7FC-0DF56B930EBE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A59AE43-B9A2-BB48-B94A-EF856CC866C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3200" yWindow="2260" windowWidth="19200" windowHeight="10680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,13 +69,13 @@
     <t>21h 45m</t>
   </si>
   <si>
-    <t>28h 50m</t>
-  </si>
-  <si>
     <t>27h 37m</t>
   </si>
   <si>
-    <t>59h 35m</t>
+    <t>60h 35m</t>
+  </si>
+  <si>
+    <t>29h 50m</t>
   </si>
 </sst>
 </file>
@@ -448,7 +448,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -474,7 +474,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -482,7 +482,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -490,7 +490,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:2">

</xml_diff>

<commit_message>
Updated time card +5:40
</commit_message>
<xml_diff>
--- a/time_cards.xlsx
+++ b/time_cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AndrewCase/Repositories/C.A.R./"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A59AE43-B9A2-BB48-B94A-EF856CC866C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B75B07A-726B-2A48-B569-A7245F17B0C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3200" yWindow="2260" windowWidth="19200" windowHeight="10680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -72,10 +72,10 @@
     <t>27h 37m</t>
   </si>
   <si>
-    <t>60h 35m</t>
-  </si>
-  <si>
     <t>29h 50m</t>
+  </si>
+  <si>
+    <t>66h 20m</t>
   </si>
 </sst>
 </file>
@@ -448,7 +448,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -474,7 +474,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -482,7 +482,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:2">

</xml_diff>

<commit_message>
Updated time card +:20
</commit_message>
<xml_diff>
--- a/time_cards.xlsx
+++ b/time_cards.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Desktop\C.A.R\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AndrewCase/Repositories/C.A.R./"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126E207E-AD78-4D4E-9C97-B2391462861A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A61C6AF5-3852-974B-918A-5CE3716AD0C0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13163" yWindow="450" windowWidth="9337" windowHeight="12150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3200" yWindow="2260" windowWidth="19200" windowHeight="10680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -72,17 +72,17 @@
     <t>29h 50m</t>
   </si>
   <si>
-    <t>66h 20m</t>
-  </si>
-  <si>
     <t>29h 52m</t>
+  </si>
+  <si>
+    <t>66h 40m</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -448,20 +448,20 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2" ht="16">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -469,15 +469,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -485,15 +485,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -501,7 +501,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -509,7 +509,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -517,7 +517,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
     </row>

</xml_diff>

<commit_message>
Updated timecard +8:25 hours
</commit_message>
<xml_diff>
--- a/time_cards.xlsx
+++ b/time_cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AndrewCase/Repositories/C.A.R./"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A61C6AF5-3852-974B-918A-5CE3716AD0C0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75CB46E6-4F69-604D-A1F5-9E2F574848AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3200" yWindow="2260" windowWidth="19200" windowHeight="10680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,7 +75,7 @@
     <t>29h 52m</t>
   </si>
   <si>
-    <t>66h 40m</t>
+    <t>75h 05m</t>
   </si>
 </sst>
 </file>
@@ -448,7 +448,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Added User Manual and updated time card
</commit_message>
<xml_diff>
--- a/time_cards.xlsx
+++ b/time_cards.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\SoftwareProject\C.A.R\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stevie_damrel/Desktop/SE1P/C.A.R./"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F25949AA-19C3-4E9E-9E16-F011385CFA13}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E214F9-DB21-9647-A8A4-192BAA9FE2D6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3520" yWindow="3520" windowWidth="21600" windowHeight="12740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,9 +63,6 @@
     <t>27h 14m</t>
   </si>
   <si>
-    <t>19h 30m</t>
-  </si>
-  <si>
     <t>21h 45m</t>
   </si>
   <si>
@@ -76,6 +73,9 @@
   </si>
   <si>
     <t>34h 17m</t>
+  </si>
+  <si>
+    <t>24h 30m</t>
   </si>
 </sst>
 </file>
@@ -448,20 +448,20 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="18.28515625" customWidth="1"/>
+    <col min="1" max="2" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -469,47 +469,47 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -517,7 +517,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
     </row>

</xml_diff>

<commit_message>
Updated timecard +1:00 Working on reformatting code, logger, & javadocs Added icon on every JOptionPane
</commit_message>
<xml_diff>
--- a/time_cards.xlsx
+++ b/time_cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AndrewCase/Repositories/C.A.R./"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2866015E-35B3-7243-A928-0815D296D755}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{813780A2-5CE9-3B45-8F68-FE916D8FF851}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3200" yWindow="2260" windowWidth="19200" windowHeight="10680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,7 +75,7 @@
     <t>24h 30m</t>
   </si>
   <si>
-    <t>75h 45m</t>
+    <t>76h 45m</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Updated timecard +2.5 hours
</commit_message>
<xml_diff>
--- a/time_cards.xlsx
+++ b/time_cards.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AndrewCase/Repositories/C.A.R./"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{813780A2-5CE9-3B45-8F68-FE916D8FF851}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5372A3E7-C79D-3B4F-8350-B72B5C454A9F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3200" yWindow="2260" windowWidth="19200" windowHeight="10680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,7 +75,7 @@
     <t>24h 30m</t>
   </si>
   <si>
-    <t>76h 45m</t>
+    <t>79h 15m</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Updated timecard +5.5 hours
</commit_message>
<xml_diff>
--- a/time_cards.xlsx
+++ b/time_cards.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\C.A.R\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AndrewCase/Repositories/C.A.R./"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC3D772C-380D-4139-96EB-149FB9EF50F6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BBFCC4F-BDE5-6E4B-A63E-13492CA0B8B6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10530" yWindow="5385" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3200" yWindow="2260" windowWidth="19200" windowHeight="10680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -72,17 +72,17 @@
     <t>24h 30m</t>
   </si>
   <si>
-    <t>79h 15m</t>
-  </si>
-  <si>
     <t>43h 01m</t>
+  </si>
+  <si>
+    <t>84h 45m</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -448,20 +448,20 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="18.28515625" customWidth="1"/>
+    <col min="1" max="2" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -469,15 +469,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -485,7 +485,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -493,7 +493,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -501,7 +501,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -509,15 +509,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
     </row>

</xml_diff>

<commit_message>
Updated time card and added powerpoint
</commit_message>
<xml_diff>
--- a/time_cards.xlsx
+++ b/time_cards.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AndrewCase/Repositories/C.A.R./"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/Desktop/Code/CSI-3471/Project/C.A.R./"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BBFCC4F-BDE5-6E4B-A63E-13492CA0B8B6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB4D42BD-1CA4-BA4A-A50E-749B7416A6CF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3200" yWindow="2260" windowWidth="19200" windowHeight="10680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,9 +63,6 @@
     <t>21h 45m</t>
   </si>
   <si>
-    <t>29h 50m</t>
-  </si>
-  <si>
     <t>34h 17m</t>
   </si>
   <si>
@@ -76,13 +73,16 @@
   </si>
   <si>
     <t>84h 45m</t>
+  </si>
+  <si>
+    <t>36h 33m</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -448,20 +448,20 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16">
+    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -469,31 +469,31 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -501,23 +501,23 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
     </row>

</xml_diff>

<commit_message>
Updated time card +:30
</commit_message>
<xml_diff>
--- a/time_cards.xlsx
+++ b/time_cards.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/Desktop/Code/CSI-3471/Project/C.A.R./"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AndrewCase/Repositories/C.A.R./"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2094AD58-9869-6C4D-A5FE-9515C1E3A4E3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D539062C-6F2C-9945-9ED9-F3BF7468FBBB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3200" yWindow="2260" windowWidth="19200" windowHeight="10680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -72,17 +72,17 @@
     <t>43h 01m</t>
   </si>
   <si>
-    <t>84h 45m</t>
-  </si>
-  <si>
     <t>36h 33m</t>
+  </si>
+  <si>
+    <t>85h 15m</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -448,20 +448,20 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="16">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -469,23 +469,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -493,7 +493,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -501,7 +501,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -509,7 +509,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -517,7 +517,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
     </row>

</xml_diff>

<commit_message>
Updated powerpoint, created iteration3 pdf, uploaded video link in website
</commit_message>
<xml_diff>
--- a/time_cards.xlsx
+++ b/time_cards.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AndrewCase/Repositories/C.A.R./"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Desktop\C.A.R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D539062C-6F2C-9945-9ED9-F3BF7468FBBB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04CD7EA8-6900-4659-9FF1-40F909196855}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="2260" windowWidth="19200" windowHeight="10680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,12 +63,6 @@
     <t>21h 45m</t>
   </si>
   <si>
-    <t>34h 17m</t>
-  </si>
-  <si>
-    <t>24h 30m</t>
-  </si>
-  <si>
     <t>43h 01m</t>
   </si>
   <si>
@@ -76,13 +70,19 @@
   </si>
   <si>
     <t>85h 15m</t>
+  </si>
+  <si>
+    <t>42h 31m</t>
+  </si>
+  <si>
+    <t>31h 30m</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -448,20 +448,20 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="2" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16">
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -469,31 +469,31 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -501,23 +501,23 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
     </row>

</xml_diff>